<commit_message>
most of template code for data_type 1 (simple layout)
</commit_message>
<xml_diff>
--- a/template/Example_input/type_1_data.xlsx
+++ b/template/Example_input/type_1_data.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\11-1-1\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\template\Example_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0108726-A289-4FE7-A5D0-2D137D72CE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C862AA-E36B-48DF-BF44-5FB10CF884D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="915" windowWidth="21600" windowHeight="11145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5340" yWindow="915" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2008" sheetId="1" r:id="rId1"/>
+    <sheet name="metadata_included" sheetId="1" r:id="rId1"/>
+    <sheet name="no_metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'2008'!$A$1:$H$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">metadata_included!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>all households
 in group (000s)</t>
@@ -55,9 +56,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>Example table</t>
-  </si>
-  <si>
     <t>Sex (head of household)</t>
   </si>
   <si>
@@ -65,12 +63,6 @@
   </si>
   <si>
     <t>Source: some source</t>
-  </si>
-  <si>
-    <t>Other series</t>
-  </si>
-  <si>
-    <t>series A</t>
   </si>
   <si>
     <t>series B</t>
@@ -115,6 +107,21 @@
   <si>
     <t>Year</t>
   </si>
+  <si>
+    <t xml:space="preserve">Other series </t>
+  </si>
+  <si>
+    <t>series    A</t>
+  </si>
+  <si>
+    <t>Example table, UK</t>
+  </si>
+  <si>
+    <t>series                     A</t>
+  </si>
+  <si>
+    <t>...Other. series …..........</t>
+  </si>
 </sst>
 </file>
 
@@ -122,7 +129,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#.0"/>
-    <numFmt numFmtId="167" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
+    <numFmt numFmtId="165" formatCode="&quot; &quot;#,##0.00&quot; &quot;;&quot;-&quot;#,##0.00&quot; &quot;;&quot; -&quot;00&quot; &quot;;&quot; &quot;@&quot; &quot;"/>
   </numFmts>
   <fonts count="28" x14ac:knownFonts="1">
     <font>
@@ -576,7 +583,7 @@
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -618,8 +625,8 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
@@ -682,9 +689,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -693,6 +697,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1060,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1084,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
@@ -1101,28 +1108,28 @@
     </row>
     <row r="3" spans="1:19" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>14</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>0</v>
@@ -1136,7 +1143,7 @@
         <v>2008</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>2</v>
@@ -1175,7 +1182,7 @@
         <v>2008</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>3</v>
@@ -1217,7 +1224,7 @@
         <v>4</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="19">
         <v>34.633903463496182</v>
@@ -1256,7 +1263,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="19">
         <v>42.283803571787871</v>
@@ -1292,10 +1299,10 @@
         <v>2008</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="26">
         <v>36.439697566238564</v>
@@ -1327,30 +1334,30 @@
       <c r="Q8" s="10"/>
     </row>
     <row r="9" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
+      <c r="A9" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
     </row>
     <row r="10" spans="1:19" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="30"/>
+      <c r="A10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="28"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
       <c r="K10" s="7"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
@@ -1411,4 +1418,249 @@
   <pageSetup paperSize="9" scale="72" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F9E8A74-6BE5-4EB3-AE88-7D27B29F6CC0}">
+  <dimension ref="A1:S8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="19">
+        <v>35.687432872156251</v>
+      </c>
+      <c r="E2" s="19">
+        <v>24.491137900784434</v>
+      </c>
+      <c r="F2" s="19">
+        <v>6.3442775991509466</v>
+      </c>
+      <c r="G2" s="20">
+        <v>2.0728423385407071</v>
+      </c>
+      <c r="H2" s="19">
+        <v>11.749701014909354</v>
+      </c>
+      <c r="I2" s="21">
+        <v>4545.1054000000022</v>
+      </c>
+      <c r="J2" s="22">
+        <v>2766.7874999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="19">
+        <v>33.517168714042498</v>
+      </c>
+      <c r="E3" s="19">
+        <v>23.584647331401921</v>
+      </c>
+      <c r="F3" s="19">
+        <v>5.2289049604446047</v>
+      </c>
+      <c r="G3" s="20">
+        <v>2.8346748614418931</v>
+      </c>
+      <c r="H3" s="19">
+        <v>11.711243121883102</v>
+      </c>
+      <c r="I3" s="21">
+        <v>3798.5778500000019</v>
+      </c>
+      <c r="J3" s="22">
+        <v>2796.8249999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19">
+        <v>34.633903463496182</v>
+      </c>
+      <c r="E4" s="19">
+        <v>20.511691524579057</v>
+      </c>
+      <c r="F4" s="19">
+        <v>7.7073087601893624</v>
+      </c>
+      <c r="G4" s="20">
+        <v>4.0457569501299195</v>
+      </c>
+      <c r="H4" s="19">
+        <v>12.325848965934556</v>
+      </c>
+      <c r="I4" s="21">
+        <v>1562.673125</v>
+      </c>
+      <c r="J4" s="22">
+        <v>1664.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="19">
+        <v>42.283803571787871</v>
+      </c>
+      <c r="E5" s="19">
+        <v>28.111803125451569</v>
+      </c>
+      <c r="F5" s="19">
+        <v>9.7809324160268876</v>
+      </c>
+      <c r="G5" s="20">
+        <v>4.8268373720060556</v>
+      </c>
+      <c r="H5" s="19">
+        <v>13.805761549103991</v>
+      </c>
+      <c r="I5" s="21">
+        <v>1824.5211375000008</v>
+      </c>
+      <c r="J5" s="22">
+        <v>1342.7874999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>2008</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="26">
+        <v>36.439697566238564</v>
+      </c>
+      <c r="E6" s="26">
+        <v>23.676706606594184</v>
+      </c>
+      <c r="F6" s="26">
+        <v>6.7236061638606213</v>
+      </c>
+      <c r="G6" s="26">
+        <v>3.7141827250630759</v>
+      </c>
+      <c r="H6" s="26">
+        <v>13.840951035101121</v>
+      </c>
+      <c r="I6" s="21">
+        <v>23815.287499999999</v>
+      </c>
+      <c r="J6" s="22">
+        <v>17269.337499999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+    </row>
+    <row r="8" spans="1:19" s="6" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="28"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:I7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
always the same regardless of header row number
</commit_message>
<xml_diff>
--- a/template/Example_input/type_1_data.xlsx
+++ b/template/Example_input/type_1_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\template\Example_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C862AA-E36B-48DF-BF44-5FB10CF884D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F21FAE-784C-4D43-B8D3-88774B8CE8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="915" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3210" yWindow="2310" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_included" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="22">
   <si>
     <t>all households
 in group (000s)</t>
@@ -108,12 +108,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">Other series </t>
-  </si>
-  <si>
-    <t>series    A</t>
-  </si>
-  <si>
     <t>Example table, UK</t>
   </si>
   <si>
@@ -121,6 +115,31 @@
   </si>
   <si>
     <t>...Other. series …..........</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex </t>
+  </si>
+  <si>
+    <r>
+      <t>Age</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <t>all households
+(000s)</t>
+  </si>
+  <si>
+    <t>sample size all households (unweighted)</t>
   </si>
 </sst>
 </file>
@@ -319,7 +338,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,12 +475,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -633,74 +646,73 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="47" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="24" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="23" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="24" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="23" fillId="24" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1068,347 +1080,298 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="4" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="7" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" style="4" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="19.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="1" customWidth="1"/>
+    <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="7" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" style="22" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="22" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="25"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="25"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2008</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="7">
         <v>35.687432872156251</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="7">
         <v>24.491137900784434</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="7">
         <v>6.3442775991509466</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="8">
         <v>2.0728423385407071</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="7">
         <v>11.749701014909354</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="9">
         <v>4545.1054000000022</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="10">
         <v>2766.7874999999995</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+    </row>
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2008</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="7">
         <v>33.517168714042498</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="7">
         <v>23.584647331401921</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="7">
         <v>5.2289049604446047</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="8">
         <v>2.8346748614418931</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="7">
         <v>11.711243121883102</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="9">
         <v>3798.5778500000019</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="10">
         <v>2796.8249999999998</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-    </row>
-    <row r="6" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    </row>
+    <row r="6" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2008</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="7">
         <v>34.633903463496182</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="7">
         <v>20.511691524579057</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="7">
         <v>7.7073087601893624</v>
       </c>
-      <c r="G6" s="20">
+      <c r="G6" s="8">
         <v>4.0457569501299195</v>
       </c>
-      <c r="H6" s="19">
+      <c r="H6" s="7">
         <v>12.325848965934556</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="9">
         <v>1562.673125</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="10">
         <v>1664.3</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-    </row>
-    <row r="7" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+    </row>
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>2008</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="19">
+      <c r="D7" s="7">
         <v>42.283803571787871</v>
       </c>
-      <c r="E7" s="19">
+      <c r="E7" s="7">
         <v>28.111803125451569</v>
       </c>
-      <c r="F7" s="19">
+      <c r="F7" s="7">
         <v>9.7809324160268876</v>
       </c>
-      <c r="G7" s="20">
+      <c r="G7" s="8">
         <v>4.8268373720060556</v>
       </c>
-      <c r="H7" s="19">
+      <c r="H7" s="7">
         <v>13.805761549103991</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="9">
         <v>1824.5211375000008</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="10">
         <v>1342.7874999999999</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-    </row>
-    <row r="8" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+    </row>
+    <row r="8" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>2008</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="14">
         <v>36.439697566238564</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="14">
         <v>23.676706606594184</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="14">
         <v>6.7236061638606213</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="14">
         <v>3.7141827250630759</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="14">
         <v>13.840951035101121</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="9">
         <v>23815.287499999999</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="10">
         <v>17269.337499999998</v>
       </c>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
-      <c r="O8" s="10"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="10"/>
-    </row>
-    <row r="9" spans="1:19" s="4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="30" t="s">
+    </row>
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-    </row>
-    <row r="10" spans="1:19" s="6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:19" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="8"/>
-      <c r="S10" s="8"/>
-    </row>
-    <row r="11" spans="1:19" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
-      <c r="O11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="8"/>
-      <c r="S11" s="8"/>
-    </row>
-    <row r="12" spans="1:19" s="4" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="8"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="22"/>
+      <c r="S10" s="22"/>
+    </row>
+    <row r="11" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="22"/>
+      <c r="S11" s="22"/>
+    </row>
+    <row r="12" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="22"/>
+      <c r="S12" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1425,237 +1388,240 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="14" t="s">
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>2008</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="7">
         <v>35.687432872156251</v>
       </c>
-      <c r="E2" s="19">
+      <c r="E2" s="7">
         <v>24.491137900784434</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="7">
         <v>6.3442775991509466</v>
       </c>
-      <c r="G2" s="20">
+      <c r="G2" s="8">
         <v>2.0728423385407071</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="7">
         <v>11.749701014909354</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="9">
         <v>4545.1054000000022</v>
       </c>
-      <c r="J2" s="22">
+      <c r="J2" s="10">
         <v>2766.7874999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+    <row r="3" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>2008</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="7">
         <v>33.517168714042498</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="7">
         <v>23.584647331401921</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="7">
         <v>5.2289049604446047</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="8">
         <v>2.8346748614418931</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="7">
         <v>11.711243121883102</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="9">
         <v>3798.5778500000019</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="10">
         <v>2796.8249999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+    <row r="4" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>2008</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="7">
         <v>34.633903463496182</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="7">
         <v>20.511691524579057</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="7">
         <v>7.7073087601893624</v>
       </c>
-      <c r="G4" s="20">
+      <c r="G4" s="8">
         <v>4.0457569501299195</v>
       </c>
-      <c r="H4" s="19">
+      <c r="H4" s="7">
         <v>12.325848965934556</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="9">
         <v>1562.673125</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="10">
         <v>1664.3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+    <row r="5" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2008</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="7">
         <v>42.283803571787871</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="7">
         <v>28.111803125451569</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="7">
         <v>9.7809324160268876</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="8">
         <v>4.8268373720060556</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="7">
         <v>13.805761549103991</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="9">
         <v>1824.5211375000008</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="10">
         <v>1342.7874999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+    <row r="6" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>2008</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="14">
         <v>36.439697566238564</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="14">
         <v>23.676706606594184</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="14">
         <v>6.7236061638606213</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="14">
         <v>3.7141827250630759</v>
       </c>
-      <c r="H6" s="26">
+      <c r="H6" s="14">
         <v>13.840951035101121</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="9">
         <v>23815.287499999999</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="10">
         <v>17269.337499999998</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="10" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="31"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="I7" s="31"/>
-    </row>
-    <row r="8" spans="1:19" s="6" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+    </row>
+    <row r="8" spans="1:19" s="20" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="29"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="8"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="22"/>
+      <c r="S8" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
clean colnames and start to remove footnotes
</commit_message>
<xml_diff>
--- a/template/Example_input/type_1_data.xlsx
+++ b/template/Example_input/type_1_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\template\Example_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F21FAE-784C-4D43-B8D3-88774B8CE8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E6DFC-9FD1-475F-B53F-842687D94769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="2310" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,12 +44,6 @@
     <t>sample size (unweighted)</t>
   </si>
   <si>
-    <t>21 to 30</t>
-  </si>
-  <si>
-    <t>31 to 40</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -140,6 +134,12 @@
   </si>
   <si>
     <t>sample size all households (unweighted)</t>
+  </si>
+  <si>
+    <t>Over 65</t>
+  </si>
+  <si>
+    <t>Under 66</t>
   </si>
 </sst>
 </file>
@@ -679,12 +679,6 @@
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -713,6 +707,12 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1080,7 +1080,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C4" sqref="C4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1090,65 +1090,65 @@
     <col min="3" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="7" style="1" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="22" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="22"/>
+    <col min="9" max="9" width="14.140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" style="20" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="25"/>
+      <c r="A1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="25"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="23"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="J3" s="4" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1156,10 +1156,10 @@
         <v>2008</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D4" s="7">
         <v>35.687432872156251</v>
@@ -1188,10 +1188,10 @@
         <v>2008</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D5" s="7">
         <v>33.517168714042498</v>
@@ -1220,10 +1220,10 @@
         <v>2008</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="7">
         <v>34.633903463496182</v>
@@ -1252,10 +1252,10 @@
         <v>2008</v>
       </c>
       <c r="B7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="D7" s="7">
         <v>42.283803571787871</v>
@@ -1284,10 +1284,10 @@
         <v>2008</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="14">
         <v>36.439697566238564</v>
@@ -1312,66 +1312,66 @@
       </c>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="1:19" s="20" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
+      <c r="A9" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+    </row>
+    <row r="10" spans="1:19" s="18" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="20"/>
     </row>
     <row r="11" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="29"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="22"/>
-      <c r="S11" s="22"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="27"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="20"/>
     </row>
     <row r="12" spans="1:19" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
+      <c r="A12" s="28"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="20"/>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,28 +1398,28 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
@@ -1433,10 +1433,10 @@
         <v>2008</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D2" s="7">
         <v>35.687432872156251</v>
@@ -1465,10 +1465,10 @@
         <v>2008</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D3" s="7">
         <v>33.517168714042498</v>
@@ -1497,10 +1497,10 @@
         <v>2008</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D4" s="7">
         <v>34.633903463496182</v>
@@ -1529,10 +1529,10 @@
         <v>2008</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>7</v>
       </c>
       <c r="D5" s="7">
         <v>42.283803571787871</v>
@@ -1561,10 +1561,10 @@
         <v>2008</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D6" s="14">
         <v>36.439697566238564</v>
@@ -1589,39 +1589,39 @@
       </c>
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:19" s="20" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="22"/>
-      <c r="N8" s="22"/>
-      <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="22"/>
-      <c r="S8" s="22"/>
+      <c r="A7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+    </row>
+    <row r="8" spans="1:19" s="18" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
template for simple excel data completed
</commit_message>
<xml_diff>
--- a/template/Example_input/type_1_data.xlsx
+++ b/template/Example_input/type_1_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding_repos\sdg_data_updates\template\Example_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7E6DFC-9FD1-475F-B53F-842687D94769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D667EF11-5AC5-4269-A7DD-85EE67CE73AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3210" yWindow="2310" windowWidth="21600" windowHeight="11145" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,15 +59,6 @@
     <t>Source: some source</t>
   </si>
   <si>
-    <t>series B</t>
-  </si>
-  <si>
-    <t>series C</t>
-  </si>
-  <si>
-    <t>series D</t>
-  </si>
-  <si>
     <r>
       <t>Age (head of household)</t>
     </r>
@@ -105,12 +96,6 @@
     <t>Example table, UK</t>
   </si>
   <si>
-    <t>series                     A</t>
-  </si>
-  <si>
-    <t>...Other. series …..........</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sex </t>
   </si>
   <si>
@@ -136,10 +121,25 @@
     <t>sample size all households (unweighted)</t>
   </si>
   <si>
-    <t>Over 65</t>
-  </si>
-  <si>
-    <t>Under 66</t>
+    <t>&lt; 66</t>
+  </si>
+  <si>
+    <t>&gt; 65</t>
+  </si>
+  <si>
+    <t>type D</t>
+  </si>
+  <si>
+    <t>type C</t>
+  </si>
+  <si>
+    <t>type B</t>
+  </si>
+  <si>
+    <t>type               A</t>
+  </si>
+  <si>
+    <t>...Other. types …..........</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1080,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C5"/>
+      <selection activeCell="D3" sqref="D3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1097,7 +1097,7 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="22"/>
@@ -1121,34 +1121,34 @@
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="I3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1159,7 +1159,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D4" s="7">
         <v>35.687432872156251</v>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D5" s="7">
         <v>33.517168714042498</v>
@@ -1313,7 +1313,7 @@
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -1388,7 +1388,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,28 +1398,28 @@
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>0</v>
@@ -1436,7 +1436,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7">
         <v>35.687432872156251</v>
@@ -1468,7 +1468,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="7">
         <v>33.517168714042498</v>
@@ -1590,7 +1590,7 @@
     </row>
     <row r="7" spans="1:19" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>

</xml_diff>